<commit_message>
Final report and analysis
</commit_message>
<xml_diff>
--- a/tendance.xlsx
+++ b/tendance.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsafr-my.sharepoint.com/personal/max_perraudin_ipsa_fr/Documents/AERO 4/S2/Ma 411 - Recherche opérationelle/TP1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipsafr-my.sharepoint.com/personal/max_perraudin_ipsa_fr/Documents/AERO 4/S2/Ma 421 - Recherche opérationelle/OP-Research PW1 KleeMintyProblem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{B56EEA59-6166-4B35-AD88-862E475B63E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C27C6E26-4332-4760-BC23-23D1C17E8B1F}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="8_{B56EEA59-6166-4B35-AD88-862E475B63E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{68925CCD-322C-4F46-A02E-F034F5875787}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CFA46FD2-F718-4028-8BA4-C50B4C66CE8A}"/>
   </bookViews>
@@ -177,6 +177,39 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Calculation Time in function of the order</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>N</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -250,11 +283,53 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.1092836832895888"/>
+                  <c:y val="6.9027777777777771E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 0.0004e</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>0.7048x</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0.9983</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -287,56 +362,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$4:$4</c:f>
+              <c:f>Sheet3!$I$4:$P$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16384"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
@@ -344,56 +395,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$3:$3</c:f>
+              <c:f>Sheet3!$I$3:$P$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16384"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.9994716644287101E-3</c:v>
+                  <c:v>0.45610451698303223</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0218315124511719E-3</c:v>
+                  <c:v>0.89541053771972656</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0013275146484375E-3</c:v>
+                  <c:v>1.8917887210845947</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1983633041381836E-2</c:v>
+                  <c:v>4.1154475212097168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2288312911987305E-2</c:v>
+                  <c:v>6.4935946464538574</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5733680725097656E-2</c:v>
+                  <c:v>16.134917497634888</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11202454566955566</c:v>
+                  <c:v>31.130236387252808</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25205445289611816</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.45610451698303223</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.89541053771972656</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.8917887210845947</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.1154475212097168</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.4935946464538574</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16.134917497634888</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>31.130236387252808</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>63.684164285659698</c:v>
                 </c:pt>
               </c:numCache>
@@ -421,6 +448,7 @@
         <c:axId val="47850656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -608,6 +636,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of iterations in function of the order N</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -681,11 +739,53 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="poly"/>
-            <c:order val="6"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.13158005249343832"/>
+                  <c:y val="7.3657407407407408E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 0.9982e</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>0.6933x</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 1</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -718,56 +818,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$4:$4</c:f>
+              <c:f>Sheet3!$I$4:$P$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16384"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
@@ -775,56 +851,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$2:$2</c:f>
+              <c:f>Sheet3!$I$2:$P$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16384"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1023</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>2047</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>4095</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>8191</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63</c:v>
+                  <c:v>16383</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>127</c:v>
+                  <c:v>32767</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>255</c:v>
+                  <c:v>65535</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>511</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1023</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2047</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4095</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8191</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16383</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>32767</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>65535</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>131071</c:v>
                 </c:pt>
               </c:numCache>
@@ -852,6 +904,7 @@
         <c:axId val="1946114496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1039,6 +1092,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Calculation time in function of the</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> order N</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1112,10 +1195,53 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="exp"/>
+            <c:trendlineType val="power"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.10199212598425197"/>
+                  <c:y val="5.5176436278798487E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 2E-10x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>9.2949</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0.9921</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -1148,56 +1274,32 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$4:$4</c:f>
+              <c:f>Sheet3!$I$4:$P$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16384"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
@@ -1205,56 +1307,32 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$3:$3</c:f>
+              <c:f>Sheet3!$I$3:$P$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16384"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.9994716644287101E-3</c:v>
+                  <c:v>0.45610451698303223</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.0218315124511719E-3</c:v>
+                  <c:v>0.89541053771972656</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.0013275146484375E-3</c:v>
+                  <c:v>1.8917887210845947</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1983633041381836E-2</c:v>
+                  <c:v>4.1154475212097168</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2288312911987305E-2</c:v>
+                  <c:v>6.4935946464538574</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5733680725097656E-2</c:v>
+                  <c:v>16.134917497634888</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11202454566955566</c:v>
+                  <c:v>31.130236387252808</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25205445289611816</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.45610451698303223</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.89541053771972656</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.8917887210845947</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4.1154475212097168</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.4935946464538574</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>16.134917497634888</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>31.130236387252808</c:v>
-                </c:pt>
-                <c:pt idx="15">
                   <c:v>63.684164285659698</c:v>
                 </c:pt>
               </c:numCache>
@@ -1282,6 +1360,8 @@
         <c:axId val="1946107296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="18"/>
+          <c:min val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1339,6 +1419,7 @@
         <c:crossAx val="1946721584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1946721584"/>
@@ -1455,6 +1536,462 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Number</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> of iterations in function of the order N</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Nombre d'itérations</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-7.7066272965879271E-2"/>
+                  <c:y val="3.3361402741324001E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 6E-07x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="30000"/>
+                      <a:t>9.1452</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0.9943</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet3!$I$4:$P$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet3!$I$2:$P$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1023</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2047</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4095</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16383</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32767</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65535</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>131071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-20A6-4290-8804-14791E81ADE9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1946114496"/>
+        <c:axId val="46355984"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1946114496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="9"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="46355984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="46355984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1946114496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1924,6 +2461,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3473,6 +4050,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4093,6 +5186,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>815340</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>449580</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{101BF90E-6C35-4CDE-9CA2-94531EAA1DA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4542,7 +5673,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>